<commit_message>
added remove account functionality
</commit_message>
<xml_diff>
--- a/Documentation/Gantt chart project plan.csv.xlsx
+++ b/Documentation/Gantt chart project plan.csv.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Go Diet App\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{35D4A080-9DB5-4C27-B0BD-FC71CA00FAC4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D2C0A344-5619-4F44-AD56-79444056B209}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt chart project plan PROGRE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="167" uniqueCount="51">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="56" uniqueCount="51">
   <si>
     <t>Phase Name</t>
   </si>
@@ -678,6 +678,33 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="21" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -687,34 +714,7 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="15" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="8" xfId="40" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5747,8 +5747,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C7" activeCellId="3" sqref="C4 C5 C6 C7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -5780,20 +5780,20 @@
       </c>
     </row>
     <row r="3" spans="2:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="9" t="d">
+      <c r="D3" s="12" t="d">
         <f>DATE(2018, 10, 1)</f>
         <v>2018-10-01</v>
       </c>
       <c r="E3" s="11">
         <v>20</v>
       </c>
-      <c r="F3" s="9" t="d">
+      <c r="F3" s="12" t="d">
         <f>D3+E3</f>
         <v>2018-10-21</v>
       </c>
@@ -5802,170 +5802,170 @@
       </c>
     </row>
     <row r="4" spans="2:7" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="16" t="s">
+      <c r="B4" s="13"/>
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="9"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="13"/>
+      <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="9"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="9"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="16" t="s">
+      <c r="B6" s="13"/>
+      <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="9"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="9"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="16" t="s">
+      <c r="B7" s="13"/>
+      <c r="C7" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="10" t="d">
+      <c r="D7" s="4" t="d">
         <f>DATE(2018, 10, 1)</f>
         <v>2018-10-01</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="5">
         <v>20</v>
       </c>
-      <c r="F7" s="10" t="d">
+      <c r="F7" s="4" t="d">
         <f>D7+E7</f>
         <v>2018-10-21</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="7" t="d">
+      <c r="D8" s="10" t="d">
         <f>DATE(2018, 10, 22)</f>
         <v>2018-10-22</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="9">
         <v>14</v>
       </c>
-      <c r="F8" s="7" t="d">
+      <c r="F8" s="10" t="d">
         <f>D8+E8</f>
         <v>2018-11-05</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="5"/>
-      <c r="C10" s="15" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="7" t="d">
+      <c r="D11" s="10" t="d">
         <f>DATE(2018, 11, 4)</f>
         <v>2018-11-04</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="9">
         <v>7</v>
       </c>
-      <c r="F11" s="7" t="d">
+      <c r="F11" s="10" t="d">
         <f>D11+E11</f>
         <v>2018-11-11</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="5"/>
-      <c r="C12" s="15" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="5"/>
-      <c r="C14" s="15" t="s">
+      <c r="B14" s="14"/>
+      <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="7" t="d">
+      <c r="D14" s="10" t="d">
         <f>DATE(2018, 11, 12)</f>
         <v>2018-11-12</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="9">
         <v>7</v>
       </c>
-      <c r="F14" s="7" t="d">
+      <c r="F14" s="10" t="d">
         <f>D14+E14</f>
         <v>2018-11-19</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="5"/>
-      <c r="C15" s="15" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="5"/>
-      <c r="C16" s="15" t="s">
+      <c r="B16" s="14"/>
+      <c r="C16" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="3" t="d">
@@ -5984,107 +5984,107 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="7" t="d">
+      <c r="D17" s="10" t="d">
         <f>DATE(2018, 11, 26)</f>
         <v>2018-11-26</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="9">
         <v>14</v>
       </c>
-      <c r="F17" s="7" t="d">
+      <c r="F17" s="10" t="d">
         <f>D17+E17</f>
         <v>2018-12-10</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="5"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="7" t="d">
+      <c r="D20" s="10" t="d">
         <f>DATE(2018, 11, 26)</f>
         <v>2018-11-26</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="9">
         <v>7</v>
       </c>
-      <c r="F20" s="7" t="d">
+      <c r="F20" s="10" t="d">
         <f>D20+E20</f>
         <v>2018-12-03</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="5"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7" t="d">
+      <c r="D22" s="10" t="d">
         <f>DATE(2018, 12, 10)</f>
         <v>2018-12-10</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="9">
         <v>14</v>
       </c>
-      <c r="F22" s="7" t="d">
+      <c r="F22" s="10" t="d">
         <f>D22+E22</f>
         <v>2018-12-24</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="5"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
@@ -6104,7 +6104,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="15" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -6126,7 +6126,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="6"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
@@ -6146,227 +6146,227 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="6"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="7" t="d">
+      <c r="D27" s="10" t="d">
         <f>DATE(2019, 1, 7)</f>
         <v>2019-01-07</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="9">
         <v>7</v>
       </c>
-      <c r="F27" s="7" t="d">
+      <c r="F27" s="10" t="d">
         <f>D27+E27</f>
         <v>2019-01-14</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G27" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="6"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="6"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="7" t="d">
+      <c r="D29" s="10" t="d">
         <f>DATE(2019, 1, 21)</f>
         <v>2019-01-21</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="9">
         <v>14</v>
       </c>
-      <c r="F29" s="7" t="d">
+      <c r="F29" s="10" t="d">
         <f>D29+E29</f>
         <v>2019-02-04</v>
       </c>
-      <c r="G29" s="8">
+      <c r="G29" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="6"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="6"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="6"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="6"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="7" t="d">
+      <c r="D33" s="10" t="d">
         <f>DATE(2019, 2, 4)</f>
         <v>2019-02-04</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="9">
         <v>7</v>
       </c>
-      <c r="F33" s="7" t="d">
+      <c r="F33" s="10" t="d">
         <f>D33+E33</f>
         <v>2019-02-11</v>
       </c>
-      <c r="G33" s="8">
+      <c r="G33" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="6"/>
+      <c r="B34" s="15"/>
       <c r="C34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="6"/>
+      <c r="B35" s="15"/>
       <c r="C35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="6"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="7" t="d">
+      <c r="D36" s="10" t="d">
         <f>DATE(2019, 2, 11)</f>
         <v>2019-02-11</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="9">
         <v>7</v>
       </c>
-      <c r="F36" s="7" t="d">
+      <c r="F36" s="10" t="d">
         <f>D36+E36</f>
         <v>2019-02-18</v>
       </c>
-      <c r="G36" s="8">
+      <c r="G36" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="6"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="7"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B38" s="6"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="6"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="7" t="d">
+      <c r="D39" s="10" t="d">
         <f>DATE(2019, 2, 18)</f>
         <v>2019-02-18</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="9">
         <v>7</v>
       </c>
-      <c r="F39" s="7" t="d">
+      <c r="F39" s="10" t="d">
         <f>D39+E39</f>
         <v>2019-02-25</v>
       </c>
-      <c r="G39" s="8">
+      <c r="G39" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B40" s="6"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="6"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="7" t="d">
+      <c r="D41" s="10" t="d">
         <f>DATE(2019, 2, 22)</f>
         <v>2019-02-22</v>
       </c>
-      <c r="E41" s="8">
+      <c r="E41" s="9">
         <v>30</v>
       </c>
-      <c r="F41" s="7" t="d">
+      <c r="F41" s="10" t="d">
         <f>D41+E41</f>
         <v>2019-03-24</v>
       </c>
-      <c r="G41" s="8">
+      <c r="G41" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="6"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="6"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="2" t="s">
         <v>41</v>
       </c>
@@ -6386,120 +6386,77 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="6"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="7" t="d">
+      <c r="D44" s="10" t="d">
         <f>DATE(2019, 2, 28)</f>
         <v>2019-02-28</v>
       </c>
-      <c r="E44" s="8">
+      <c r="E44" s="9">
         <v>30</v>
       </c>
-      <c r="F44" s="7" t="d">
+      <c r="F44" s="10" t="d">
         <f>DATE(2019, 4, 5)</f>
         <v>2019-04-05</v>
       </c>
-      <c r="G44" s="8">
+      <c r="G44" s="9">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="6"/>
+      <c r="B45" s="15"/>
       <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B46" s="6"/>
+      <c r="B46" s="15"/>
       <c r="C46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="7"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="6"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D47" s="7"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="6"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="7"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="6"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="F44:F49"/>
-    <mergeCell ref="G44:G49"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B8:B24"/>
     <mergeCell ref="B25:B49"/>
@@ -6516,6 +6473,49 @@
     <mergeCell ref="D44:D49"/>
     <mergeCell ref="E44:E49"/>
     <mergeCell ref="E39:E40"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="F44:F49"/>
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added diagram, User Sequence diagrams/UserSequenceDiagram.graphml, fixed database
</commit_message>
<xml_diff>
--- a/Documentation/Gantt chart project plan.csv.xlsx
+++ b/Documentation/Gantt chart project plan.csv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\Go Diet App\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D2C0A344-5619-4F44-AD56-79444056B209}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0C86A519-9E01-44E1-86C5-806BE7CC9FA2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -693,17 +693,8 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="8" xfId="40" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="21" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -714,7 +705,16 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="19" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="8" xfId="40" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="5" borderId="4" xfId="9" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5747,8 +5747,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C24" activeCellId="2" sqref="C22 C23 C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -5780,59 +5780,59 @@
       </c>
     </row>
     <row r="3" spans="2:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="d">
+      <c r="D3" s="13" t="d">
         <f>DATE(2018, 10, 1)</f>
         <v>2018-10-01</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="14">
         <v>20</v>
       </c>
-      <c r="F3" s="12" t="d">
+      <c r="F3" s="13" t="d">
         <f>D3+E3</f>
         <v>2018-10-21</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="14"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="13"/>
+      <c r="B5" s="10"/>
       <c r="C5" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="11"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="8" t="s">
         <v>48</v>
       </c>
@@ -5852,120 +5852,120 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10" t="d">
+      <c r="D8" s="15" t="d">
         <f>DATE(2018, 10, 22)</f>
         <v>2018-10-22</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="16">
         <v>14</v>
       </c>
-      <c r="F8" s="10" t="d">
+      <c r="F8" s="15" t="d">
         <f>D8+E8</f>
         <v>2018-11-05</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="14"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="14"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="9"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B11" s="14"/>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10" t="d">
+      <c r="D11" s="15" t="d">
         <f>DATE(2018, 11, 4)</f>
         <v>2018-11-04</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="16">
         <v>7</v>
       </c>
-      <c r="F11" s="10" t="d">
+      <c r="F11" s="15" t="d">
         <f>D11+E11</f>
         <v>2018-11-11</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="14"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="9"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="14"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="9"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B14" s="14"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="10" t="d">
+      <c r="D14" s="15" t="d">
         <f>DATE(2018, 11, 12)</f>
         <v>2018-11-12</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="16">
         <v>7</v>
       </c>
-      <c r="F14" s="10" t="d">
+      <c r="F14" s="15" t="d">
         <f>D14+E14</f>
         <v>2018-11-19</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="14"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="9"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B16" s="14"/>
-      <c r="C16" s="7" t="s">
+      <c r="B16" s="11"/>
+      <c r="C16" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D16" s="3" t="d">
@@ -5984,108 +5984,108 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="14"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="10" t="d">
+      <c r="D17" s="15" t="d">
         <f>DATE(2018, 11, 26)</f>
         <v>2018-11-26</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="16">
         <v>14</v>
       </c>
-      <c r="F17" s="10" t="d">
+      <c r="F17" s="15" t="d">
         <f>D17+E17</f>
         <v>2018-12-10</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="14"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="14"/>
-      <c r="C19" s="2" t="s">
+      <c r="B19" s="11"/>
+      <c r="C19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="9"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="14"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="10" t="d">
+      <c r="D20" s="15" t="d">
         <f>DATE(2018, 11, 26)</f>
         <v>2018-11-26</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="16">
         <v>7</v>
       </c>
-      <c r="F20" s="10" t="d">
+      <c r="F20" s="15" t="d">
         <f>D20+E20</f>
         <v>2018-12-03</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="14"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="9"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="14"/>
-      <c r="C22" s="2" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="10" t="d">
+      <c r="D22" s="15" t="d">
         <f>DATE(2018, 12, 10)</f>
         <v>2018-12-10</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="16">
         <v>14</v>
       </c>
-      <c r="F22" s="10" t="d">
+      <c r="F22" s="15" t="d">
         <f>D22+E22</f>
         <v>2018-12-24</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B23" s="14"/>
-      <c r="C23" s="2" t="s">
+      <c r="B23" s="11"/>
+      <c r="C23" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="9"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="14"/>
-      <c r="C24" s="2" t="s">
+      <c r="B24" s="11"/>
+      <c r="C24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="3" t="d">
@@ -6104,7 +6104,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -6126,7 +6126,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="2" t="s">
         <v>27</v>
       </c>
@@ -6146,227 +6146,227 @@
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="10" t="d">
+      <c r="D27" s="15" t="d">
         <f>DATE(2019, 1, 7)</f>
         <v>2019-01-07</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="16">
         <v>7</v>
       </c>
-      <c r="F27" s="10" t="d">
+      <c r="F27" s="15" t="d">
         <f>D27+E27</f>
         <v>2019-01-14</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="15"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="9"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B29" s="15"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D29" s="10" t="d">
+      <c r="D29" s="15" t="d">
         <f>DATE(2019, 1, 21)</f>
         <v>2019-01-21</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="16">
         <v>14</v>
       </c>
-      <c r="F29" s="10" t="d">
+      <c r="F29" s="15" t="d">
         <f>D29+E29</f>
         <v>2019-02-04</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B30" s="15"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="10"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="9"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="15"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="9"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="15"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="9"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="15"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="10" t="d">
+      <c r="D33" s="15" t="d">
         <f>DATE(2019, 2, 4)</f>
         <v>2019-02-04</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="16">
         <v>7</v>
       </c>
-      <c r="F33" s="10" t="d">
+      <c r="F33" s="15" t="d">
         <f>D33+E33</f>
         <v>2019-02-11</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="15"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="9"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="15"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="9"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B36" s="15"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D36" s="10" t="d">
+      <c r="D36" s="15" t="d">
         <f>DATE(2019, 2, 11)</f>
         <v>2019-02-11</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="16">
         <v>7</v>
       </c>
-      <c r="F36" s="10" t="d">
+      <c r="F36" s="15" t="d">
         <f>D36+E36</f>
         <v>2019-02-18</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B37" s="15"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="10"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="9"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="16"/>
     </row>
     <row r="38" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B38" s="15"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="10"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="9"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="16"/>
     </row>
     <row r="39" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="15"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D39" s="10" t="d">
+      <c r="D39" s="15" t="d">
         <f>DATE(2019, 2, 18)</f>
         <v>2019-02-18</v>
       </c>
-      <c r="E39" s="9">
+      <c r="E39" s="16">
         <v>7</v>
       </c>
-      <c r="F39" s="10" t="d">
+      <c r="F39" s="15" t="d">
         <f>D39+E39</f>
         <v>2019-02-25</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B40" s="15"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="10"/>
-      <c r="E40" s="9"/>
-      <c r="F40" s="10"/>
-      <c r="G40" s="9"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="15"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="10" t="d">
+      <c r="D41" s="15" t="d">
         <f>DATE(2019, 2, 22)</f>
         <v>2019-02-22</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="16">
         <v>30</v>
       </c>
-      <c r="F41" s="10" t="d">
+      <c r="F41" s="15" t="d">
         <f>D41+E41</f>
         <v>2019-03-24</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="15"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D42" s="10"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="9"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="15"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="2" t="s">
         <v>41</v>
       </c>
@@ -6386,77 +6386,120 @@
       </c>
     </row>
     <row r="44" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B44" s="15"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="10" t="d">
+      <c r="D44" s="15" t="d">
         <f>DATE(2019, 2, 28)</f>
         <v>2019-02-28</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="16">
         <v>30</v>
       </c>
-      <c r="F44" s="10" t="d">
+      <c r="F44" s="15" t="d">
         <f>DATE(2019, 4, 5)</f>
         <v>2019-04-05</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B45" s="15"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D45" s="10"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="9"/>
+      <c r="D45" s="15"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B46" s="15"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="9"/>
+      <c r="D46" s="15"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="16"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B47" s="15"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D47" s="10"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="10"/>
-      <c r="G47" s="9"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B48" s="15"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D48" s="10"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="9"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="16"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B49" s="15"/>
+      <c r="B49" s="12"/>
       <c r="C49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D49" s="10"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="10"/>
-      <c r="G49" s="9"/>
+      <c r="D49" s="15"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="59">
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="F29:F32"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="G33:G35"/>
+    <mergeCell ref="G29:G32"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="G36:G38"/>
+    <mergeCell ref="F44:F49"/>
+    <mergeCell ref="G44:G49"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B8:B24"/>
     <mergeCell ref="B25:B49"/>
@@ -6473,49 +6516,6 @@
     <mergeCell ref="D44:D49"/>
     <mergeCell ref="E44:E49"/>
     <mergeCell ref="E39:E40"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D32"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="F44:F49"/>
-    <mergeCell ref="G44:G49"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="G36:G38"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="E29:E32"/>
-    <mergeCell ref="F29:F32"/>
-    <mergeCell ref="F33:F35"/>
-    <mergeCell ref="G33:G35"/>
-    <mergeCell ref="G29:G32"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="G22:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>